<commit_message>
update default time zone
</commit_message>
<xml_diff>
--- a/stocker.xlsx
+++ b/stocker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Leveraged Free Cash Flow" sheetId="1" r:id="rId4"/>
@@ -660,7 +660,7 @@
   </sheetPr>
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -705,16 +705,16 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <v>3287000</v>
+      </c>
+      <c r="C3">
         <v>2825000</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2611000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2334000</v>
-      </c>
-      <c r="E3">
-        <v>3669000</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1079,16 +1079,16 @@
         <v>29</v>
       </c>
       <c r="B25">
+        <v>111000</v>
+      </c>
+      <c r="C25">
         <v>-2000</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>95000</v>
       </c>
-      <c r="D25">
-        <v>194000</v>
-      </c>
       <c r="E25">
-        <v>84000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1623,16 +1623,16 @@
         <v>59</v>
       </c>
       <c r="B57">
+        <v>-27214</v>
+      </c>
+      <c r="C57">
         <v>2311</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>365763</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>-21361</v>
-      </c>
-      <c r="E57">
-        <v>26232</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2082,16 +2082,16 @@
         <v>86</v>
       </c>
       <c r="B84">
+        <v>3005000</v>
+      </c>
+      <c r="C84">
         <v>3782000</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>6328000</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>-1371000</v>
-      </c>
-      <c r="E84">
-        <v>3259000</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2286,16 +2286,16 @@
         <v>98</v>
       </c>
       <c r="B96">
+        <v>66894</v>
+      </c>
+      <c r="C96">
         <v>124005</v>
       </c>
-      <c r="C96">
+      <c r="D96">
         <v>38251</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>159768</v>
-      </c>
-      <c r="E96">
-        <v>319762</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2400,16 +2400,16 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <v>52074000</v>
+      </c>
+      <c r="C3">
         <v>50469000</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>47065000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>48201000</v>
-      </c>
-      <c r="E3">
-        <v>50610000</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2774,16 +2774,16 @@
         <v>29</v>
       </c>
       <c r="B25">
+        <v>358000</v>
+      </c>
+      <c r="C25">
         <v>183000</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>430000</v>
       </c>
-      <c r="D25">
-        <v>462000</v>
-      </c>
       <c r="E25">
-        <v>563000</v>
+        <v>814000</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3318,16 +3318,16 @@
         <v>59</v>
       </c>
       <c r="B57">
+        <v>310740</v>
+      </c>
+      <c r="C57">
         <v>357122</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>600116</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>257525</v>
-      </c>
-      <c r="E57">
-        <v>335023</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3777,16 +3777,16 @@
         <v>86</v>
       </c>
       <c r="B84">
+        <v>6184000</v>
+      </c>
+      <c r="C84">
         <v>6012000</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>7281000</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>8736000</v>
-      </c>
-      <c r="E84">
-        <v>9016000</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -3981,16 +3981,16 @@
         <v>98</v>
       </c>
       <c r="B96">
+        <v>308042</v>
+      </c>
+      <c r="C96">
         <v>385790</v>
       </c>
-      <c r="C96">
+      <c r="D96">
         <v>290899</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>405709</v>
-      </c>
-      <c r="E96">
-        <v>486050</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4050,7 +4050,7 @@
   </sheetPr>
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4095,16 +4095,16 @@
         <v>6</v>
       </c>
       <c r="B3">
+        <v>20909000</v>
+      </c>
+      <c r="C3">
         <v>20892000</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>17147000</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>16226000</v>
-      </c>
-      <c r="E3">
-        <v>16211000</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4469,16 +4469,16 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>1333000</v>
+        <v>1332000</v>
       </c>
       <c r="C25">
         <v>1333000</v>
       </c>
       <c r="D25">
-        <v>1335000</v>
+        <v>1333000</v>
       </c>
       <c r="E25">
-        <v>1298000</v>
+        <v>1481000</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5013,16 +5013,16 @@
         <v>59</v>
       </c>
       <c r="B57">
+        <v>247437</v>
+      </c>
+      <c r="C57">
         <v>192941</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>195726</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>200373</v>
-      </c>
-      <c r="E57">
-        <v>203626</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -5472,16 +5472,16 @@
         <v>86</v>
       </c>
       <c r="B84">
+        <v>54175000</v>
+      </c>
+      <c r="C84">
         <v>55545000</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>56641000</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>61822000</v>
-      </c>
-      <c r="E84">
-        <v>57225000</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -5676,16 +5676,16 @@
         <v>98</v>
       </c>
       <c r="B96">
+        <v>1269495</v>
+      </c>
+      <c r="C96">
         <v>1289661</v>
       </c>
-      <c r="C96">
+      <c r="D96">
         <v>1302230</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>1315596</v>
-      </c>
-      <c r="E96">
-        <v>1329508</v>
       </c>
     </row>
     <row r="97" spans="1:5">

</xml_diff>